<commit_message>
domingo de trabajo wtf
</commit_message>
<xml_diff>
--- a/assets uarm/2019 sol-penscri-justfilpol/injusticia absoluta de la validación cognitiva.xlsx
+++ b/assets uarm/2019 sol-penscri-justfilpol/injusticia absoluta de la validación cognitiva.xlsx
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B16" sqref="B5:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f>SUM(E20:H20)</f>
+        <f t="shared" ref="I20:I25" si="0">SUM(E20:H20)</f>
         <v>13</v>
       </c>
     </row>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <f>SUM(E21:H21)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="I22">
-        <f>SUM(E22:H22)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -907,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="I23">
-        <f>SUM(E23:H23)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -928,7 +928,7 @@
         <v>2</v>
       </c>
       <c r="I24">
-        <f>SUM(E24:H24)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="I25">
-        <f>SUM(E25:H25)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <f>SUM(E29:H29)</f>
+        <f t="shared" ref="I29:I35" si="1">SUM(E29:H29)</f>
         <v>16</v>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="I30">
-        <f>SUM(E30:H30)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="I31">
-        <f>SUM(E31:H31)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <f>SUM(E32:H32)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="I33">
-        <f>SUM(E33:H33)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="I34">
-        <f>SUM(E34:H34)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="I35">
-        <f>SUM(E35:H35)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>

</xml_diff>